<commit_message>
Revised labels for design power levels for consistency with E+ IDF
</commit_message>
<xml_diff>
--- a/design/Commercial/Medium Office/ASHRAE 90.1-2019/Medium Office - ASHRAE 90.1-2019 - Connected Plug Loads.xlsx
+++ b/design/Commercial/Medium Office/ASHRAE 90.1-2019/Medium Office - ASHRAE 90.1-2019 - Connected Plug Loads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfrank1\Git\prototype-building-electrical-models\design\Commercial\Medium Office\ASHRAE 90.1-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD8CF1F-A15A-4460-B107-63700C159F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FB149C-2EF3-41DC-8B4B-45AC5FE7BE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Floor 1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{210542B0-9181-4F05-921F-E0F7B96DC27C}">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{77696BDC-802E-4F12-ADFB-0BA38884A637}">
       <text>
         <r>
           <rPr>
@@ -531,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{B304B2E1-BE7B-4BD3-9715-9B2B8AB79180}">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{1E48C475-8E4C-4FDE-BC9A-2CB423D5F7C1}">
       <text>
         <r>
           <rPr>
@@ -818,12 +818,6 @@
     </r>
   </si>
   <si>
-    <t>Effective Load (W)</t>
-  </si>
-  <si>
-    <t>Effective Load:</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -831,6 +825,12 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Design Power Level:</t>
+  </si>
+  <si>
+    <t>Design Load (W)</t>
   </si>
 </sst>
 </file>
@@ -1187,6 +1187,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1234,63 +1291,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1816,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,60 +1830,60 @@
     <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="46"/>
+      <c r="C6" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="65"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -1895,7 +1895,7 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -1907,7 +1907,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -1927,7 +1927,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -1950,75 +1950,75 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="2:12" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+    </row>
+    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="64" t="s">
+      <c r="G17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="65" t="s">
+      <c r="I17" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="49" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="32">
         <v>0</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="33">
         <v>0</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="35">
         <v>1046</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="37">
         <v>0.115</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="35">
         <f>F18*D18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="51">
+      <c r="I18" s="35">
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="36" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
         <v>2.81</v>
       </c>
       <c r="D19" s="10">
-        <f>ROUND(C19*($C$10/1000),0)</f>
+        <f t="shared" ref="D19:D24" si="0">ROUND(C19*($C$10/1000),0)</f>
         <v>50</v>
       </c>
       <c r="E19" s="21">
@@ -2040,15 +2040,15 @@
       <c r="F19" s="28">
         <v>57</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="38">
         <v>0.32200000000000001</v>
       </c>
       <c r="H19" s="28">
-        <f t="shared" ref="H19:H25" si="0">F19*D19</f>
+        <f t="shared" ref="H19:H25" si="1">F19*D19</f>
         <v>2850</v>
       </c>
       <c r="I19" s="28">
-        <f t="shared" ref="I19:I25" si="1">H19*G19</f>
+        <f t="shared" ref="I19:I25" si="2">H19*G19</f>
         <v>917.7</v>
       </c>
       <c r="J19" s="11"/>
@@ -2061,7 +2061,7 @@
         <v>1.87</v>
       </c>
       <c r="D20" s="10">
-        <f>ROUND(C20*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E20" s="21">
@@ -2070,15 +2070,15 @@
       <c r="F20" s="28">
         <v>46</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H20" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1518</v>
       </c>
       <c r="I20" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>847.0440000000001</v>
       </c>
       <c r="J20" s="11"/>
@@ -2091,7 +2091,7 @@
         <v>0.26</v>
       </c>
       <c r="D21" s="10">
-        <f>ROUND(C21*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E21" s="21">
@@ -2100,48 +2100,48 @@
       <c r="F21" s="28">
         <v>127</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H21" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
       <c r="I21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>354.33000000000004</v>
       </c>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="32">
         <v>0</v>
       </c>
-      <c r="D22" s="49">
-        <f>ROUND(C22*($C$10/1000),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="51">
-        <v>648</v>
-      </c>
-      <c r="G22" s="53">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="H22" s="51">
+      <c r="D22" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="51">
+      <c r="E22" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="35">
+        <v>648</v>
+      </c>
+      <c r="G22" s="37">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="H22" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="I22" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="36" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
         <v>0.52</v>
       </c>
       <c r="D23" s="10">
-        <f>ROUND(C23*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -2162,15 +2162,15 @@
       <c r="F23" s="28">
         <v>875</v>
       </c>
-      <c r="G23" s="54">
+      <c r="G23" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H23" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7875</v>
       </c>
       <c r="I23" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2134.125</v>
       </c>
       <c r="J23" s="11"/>
@@ -2183,7 +2183,7 @@
         <v>0.17</v>
       </c>
       <c r="D24" s="10">
-        <f>ROUND(C24*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E24" s="24" t="s">
@@ -2192,15 +2192,15 @@
       <c r="F24" s="28">
         <v>684</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H24" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2052</v>
       </c>
       <c r="I24" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>556.09199999999998</v>
       </c>
       <c r="J24" s="11"/>
@@ -2214,7 +2214,7 @@
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="2">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2224,19 +2224,19 @@
         <f>32*5</f>
         <v>160</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="38">
         <v>0.22500000000000001</v>
       </c>
       <c r="H25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8800</v>
       </c>
       <c r="I25" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1980</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2263,26 +2263,26 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57">
+      <c r="B27" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41">
         <f>SUM(D18:D26)</f>
         <v>405</v>
       </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59">
-        <f t="shared" ref="H27:I27" si="3">SUM(H18:H26)</f>
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43">
+        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
-      <c r="I27" s="59">
-        <f t="shared" si="3"/>
+      <c r="I27" s="43">
+        <f t="shared" si="4"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="60"/>
+      <c r="J27" s="44"/>
       <c r="L27" s="1"/>
     </row>
   </sheetData>
@@ -2347,7 +2347,7 @@
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,60 +2360,60 @@
     <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="46"/>
+      <c r="C6" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="65"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -2425,7 +2425,7 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -2480,75 +2480,75 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="2:12" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+    </row>
+    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="64" t="s">
+      <c r="G17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="65" t="s">
+      <c r="I17" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="49" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="32">
         <v>0</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="33">
         <v>0</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="35">
         <v>1046</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="37">
         <v>0.115</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="35">
         <f>F18*D18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="51">
+      <c r="I18" s="35">
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="36" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
         <v>2.81</v>
       </c>
       <c r="D19" s="10">
-        <f>ROUND(C19*($C$10/1000),0)</f>
+        <f t="shared" ref="D19:D24" si="0">ROUND(C19*($C$10/1000),0)</f>
         <v>50</v>
       </c>
       <c r="E19" s="21">
@@ -2570,15 +2570,15 @@
       <c r="F19" s="28">
         <v>57</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="38">
         <v>0.32200000000000001</v>
       </c>
       <c r="H19" s="28">
-        <f t="shared" ref="H19:H25" si="0">F19*D19</f>
+        <f t="shared" ref="H19:H25" si="1">F19*D19</f>
         <v>2850</v>
       </c>
       <c r="I19" s="28">
-        <f t="shared" ref="I19:I25" si="1">H19*G19</f>
+        <f t="shared" ref="I19:I25" si="2">H19*G19</f>
         <v>917.7</v>
       </c>
       <c r="J19" s="11"/>
@@ -2591,7 +2591,7 @@
         <v>1.87</v>
       </c>
       <c r="D20" s="10">
-        <f>ROUND(C20*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E20" s="21">
@@ -2600,15 +2600,15 @@
       <c r="F20" s="28">
         <v>46</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H20" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1518</v>
       </c>
       <c r="I20" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>847.0440000000001</v>
       </c>
       <c r="J20" s="11"/>
@@ -2621,7 +2621,7 @@
         <v>0.26</v>
       </c>
       <c r="D21" s="10">
-        <f>ROUND(C21*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E21" s="21">
@@ -2630,48 +2630,48 @@
       <c r="F21" s="28">
         <v>127</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H21" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
       <c r="I21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>354.33000000000004</v>
       </c>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="32">
         <v>0</v>
       </c>
-      <c r="D22" s="49">
-        <f>ROUND(C22*($C$10/1000),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="51">
-        <v>648</v>
-      </c>
-      <c r="G22" s="53">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="H22" s="51">
+      <c r="D22" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="51">
+      <c r="E22" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="35">
+        <v>648</v>
+      </c>
+      <c r="G22" s="37">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="H22" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="I22" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="36" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
         <v>0.52</v>
       </c>
       <c r="D23" s="10">
-        <f>ROUND(C23*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -2692,15 +2692,15 @@
       <c r="F23" s="28">
         <v>875</v>
       </c>
-      <c r="G23" s="54">
+      <c r="G23" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H23" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7875</v>
       </c>
       <c r="I23" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2134.125</v>
       </c>
       <c r="J23" s="11"/>
@@ -2713,7 +2713,7 @@
         <v>0.17</v>
       </c>
       <c r="D24" s="10">
-        <f>ROUND(C24*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E24" s="24" t="s">
@@ -2722,15 +2722,15 @@
       <c r="F24" s="28">
         <v>684</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H24" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2052</v>
       </c>
       <c r="I24" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>556.09199999999998</v>
       </c>
       <c r="J24" s="11"/>
@@ -2744,7 +2744,7 @@
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="2">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2754,19 +2754,19 @@
         <f>32*5</f>
         <v>160</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="38">
         <v>0.22500000000000001</v>
       </c>
       <c r="H25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8800</v>
       </c>
       <c r="I25" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1980</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2793,26 +2793,26 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57">
+      <c r="B27" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41">
         <f>SUM(D18:D26)</f>
         <v>646</v>
       </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59">
-        <f t="shared" ref="H27:I27" si="3">SUM(H18:H26)</f>
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43">
+        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
-      <c r="I27" s="59">
-        <f t="shared" si="3"/>
+      <c r="I27" s="43">
+        <f t="shared" si="4"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="60"/>
+      <c r="J27" s="44"/>
       <c r="L27" s="1"/>
     </row>
   </sheetData>
@@ -2876,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C792F2A7-A451-44D0-B4BC-456BE5420D34}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2890,60 +2890,60 @@
     <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="46"/>
+      <c r="C6" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="65"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -2955,7 +2955,7 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -2967,7 +2967,7 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -3010,75 +3010,75 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="2:12" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+    </row>
+    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="64" t="s">
+      <c r="G17" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="65" t="s">
+      <c r="I17" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="49" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="32">
         <v>0</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="33">
         <v>0</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="35">
         <v>1046</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="37">
         <v>0.115</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="35">
         <f>F18*D18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="51">
+      <c r="I18" s="35">
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="36" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
         <v>2.81</v>
       </c>
       <c r="D19" s="10">
-        <f>ROUND(C19*($C$10/1000),0)</f>
+        <f t="shared" ref="D19:D24" si="0">ROUND(C19*($C$10/1000),0)</f>
         <v>50</v>
       </c>
       <c r="E19" s="21">
@@ -3100,15 +3100,15 @@
       <c r="F19" s="28">
         <v>57</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="38">
         <v>0.32200000000000001</v>
       </c>
       <c r="H19" s="28">
-        <f t="shared" ref="H19:H25" si="0">F19*D19</f>
+        <f t="shared" ref="H19:H25" si="1">F19*D19</f>
         <v>2850</v>
       </c>
       <c r="I19" s="28">
-        <f t="shared" ref="I19:I25" si="1">H19*G19</f>
+        <f t="shared" ref="I19:I25" si="2">H19*G19</f>
         <v>917.7</v>
       </c>
       <c r="J19" s="11"/>
@@ -3121,7 +3121,7 @@
         <v>1.87</v>
       </c>
       <c r="D20" s="10">
-        <f>ROUND(C20*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E20" s="21">
@@ -3130,15 +3130,15 @@
       <c r="F20" s="28">
         <v>46</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H20" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1518</v>
       </c>
       <c r="I20" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>847.0440000000001</v>
       </c>
       <c r="J20" s="11"/>
@@ -3151,7 +3151,7 @@
         <v>0.26</v>
       </c>
       <c r="D21" s="10">
-        <f>ROUND(C21*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E21" s="21">
@@ -3160,48 +3160,48 @@
       <c r="F21" s="28">
         <v>127</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="38">
         <v>0.55800000000000005</v>
       </c>
       <c r="H21" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635</v>
       </c>
       <c r="I21" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>354.33000000000004</v>
       </c>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="32">
         <v>0</v>
       </c>
-      <c r="D22" s="49">
-        <f>ROUND(C22*($C$10/1000),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="51">
-        <v>648</v>
-      </c>
-      <c r="G22" s="53">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="H22" s="51">
+      <c r="D22" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="51">
+      <c r="E22" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="35">
+        <v>648</v>
+      </c>
+      <c r="G22" s="37">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="H22" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="I22" s="35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="36" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
         <v>0.52</v>
       </c>
       <c r="D23" s="10">
-        <f>ROUND(C23*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -3222,15 +3222,15 @@
       <c r="F23" s="28">
         <v>875</v>
       </c>
-      <c r="G23" s="54">
+      <c r="G23" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H23" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7875</v>
       </c>
       <c r="I23" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2134.125</v>
       </c>
       <c r="J23" s="11"/>
@@ -3243,7 +3243,7 @@
         <v>0.17</v>
       </c>
       <c r="D24" s="10">
-        <f>ROUND(C24*($C$10/1000),0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E24" s="24" t="s">
@@ -3252,15 +3252,15 @@
       <c r="F24" s="28">
         <v>684</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="38">
         <v>0.27100000000000002</v>
       </c>
       <c r="H24" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2052</v>
       </c>
       <c r="I24" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>556.09199999999998</v>
       </c>
       <c r="J24" s="11"/>
@@ -3274,7 +3274,7 @@
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="2">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -3284,19 +3284,19 @@
         <f>32*5</f>
         <v>160</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="38">
         <v>0.22500000000000001</v>
       </c>
       <c r="H25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8800</v>
       </c>
       <c r="I25" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1980</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3323,26 +3323,26 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="57">
+      <c r="B27" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41">
         <f>SUM(D18:D26)</f>
         <v>535</v>
       </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59">
-        <f t="shared" ref="H27:I27" si="3">SUM(H18:H26)</f>
+      <c r="E27" s="41"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43">
+        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
-      <c r="I27" s="59">
-        <f t="shared" si="3"/>
+      <c r="I27" s="43">
+        <f t="shared" si="4"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="60"/>
+      <c r="J27" s="44"/>
       <c r="L27" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated plug load converter sizing to reflect converter output rating, not input rating. Updated profiles to correct for demand factor and converter full load efficiency.
</commit_message>
<xml_diff>
--- a/design/Commercial/Medium Office/ASHRAE 90.1-2019/Medium Office - ASHRAE 90.1-2019 - Connected Plug Loads.xlsx
+++ b/design/Commercial/Medium Office/ASHRAE 90.1-2019/Medium Office - ASHRAE 90.1-2019 - Connected Plug Loads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfrank1\Git\prototype-building-electrical-models\design\Commercial\Medium Office\ASHRAE 90.1-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FB149C-2EF3-41DC-8B4B-45AC5FE7BE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E0844E-E652-4247-87BC-309439C76F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Floor 1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total connected load from devices is not equal to effective load from EnergyPlus due to individual load demand factors.</t>
+          <t>Total connected load from devices is not equal to design load from EnergyPlus due to individual load demand factors.</t>
         </r>
       </text>
     </comment>
@@ -199,6 +199,32 @@
             <family val="2"/>
           </rPr>
           <t>Uses device peak load instead of connected load to account for device demand factors. This column gives each device's "share" of the building's total plug load.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{69721171-FE0D-408C-9E07-4BCDA5561F4B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the full load efficiency of the representative converter model selected for the group. It is used to convert the AC (input) power rating to a DC (output) power rating.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{3142C727-BB93-4815-A149-389B0960314A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Equals rated unit input power multiplied by full load efficiency.</t>
         </r>
       </text>
     </comment>
@@ -283,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{761E9C71-A28B-4EF5-8F6D-E5F5A96D298A}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{848D8969-48DB-4AFB-B4FD-F48F9951752B}">
       <text>
         <r>
           <rPr>
@@ -347,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{FCB4CFFC-10E6-4031-B8C5-DCF1F9D76C34}">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{0CBDB54B-81A5-4E43-B5D6-A5A3399DBA3B}">
       <text>
         <r>
           <rPr>
@@ -356,7 +382,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total connected load from devices is not equal to effective load from EnergyPlus due to individual load demand factors.</t>
+          <t>Total connected load from devices is not equal to design load from EnergyPlus due to individual load demand factors.</t>
         </r>
       </text>
     </comment>
@@ -370,6 +396,32 @@
             <family val="2"/>
           </rPr>
           <t>Uses device peak load instead of connected load to account for device demand factors. This column gives each device's "share" of the building's total plug load.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{FEA69B1D-A78A-4660-9652-B6A0FD1E06C3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the full load efficiency of the representative converter model selected for the group. It is used to convert the AC (input) power rating to a DC (output) power rating.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{82CD1A78-83E2-4228-AC42-28872D2AD338}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Equals rated unit input power multiplied by full load efficiency.</t>
         </r>
       </text>
     </comment>
@@ -454,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{4BF5DCD0-F95F-4D77-89E0-D8BB3C912434}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{CB458009-F73D-4C04-9E08-6F36554FF209}">
       <text>
         <r>
           <rPr>
@@ -518,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{0A8A66B8-AACB-4B71-898D-0A3375A91EC8}">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{B1A2CFE5-8DD5-4EC4-9BBF-8B1488C0DDDC}">
       <text>
         <r>
           <rPr>
@@ -527,7 +579,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total connected load from devices is not equal to effective load from EnergyPlus due to individual load demand factors.</t>
+          <t>Total connected load from devices is not equal to design load from EnergyPlus due to individual load demand factors.</t>
         </r>
       </text>
     </comment>
@@ -541,6 +593,32 @@
             <family val="2"/>
           </rPr>
           <t>Uses device peak load instead of connected load to account for device demand factors. This column gives each device's "share" of the building's total plug load.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{1F88FE39-3D31-4FDE-95BD-DAC09703849C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the full load efficiency of the representative converter model selected for the group. It is used to convert the AC (input) power rating to a DC (output) power rating.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0" xr:uid="{56294B23-153A-48A2-BE57-52493BF9A60C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Equals rated unit input power multiplied by full load efficiency.</t>
         </r>
       </text>
     </comment>
@@ -549,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
   <si>
     <t>Device Type</t>
   </si>
@@ -729,34 +807,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Rated Unit Power (W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>rated</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Assume all desktop computers converted to laptop computers.</t>
   </si>
   <si>
@@ -832,15 +882,75 @@
   <si>
     <t>Design Load (W)</t>
   </si>
+  <si>
+    <r>
+      <t>Rated Unit Input Power (W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rated</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Full Load Efficiency (%)</t>
+  </si>
+  <si>
+    <r>
+      <t>Rated Unit Output Power (W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dc</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -887,6 +997,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -920,6 +1031,13 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1091,11 +1209,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1244,6 +1363,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1293,11 +1419,52 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{851E28D6-5DEB-4D86-A213-06EBF2C71B60}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1814,11 +1981,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L27"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1827,65 +1992,67 @@
     <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="21.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="61"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="64"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="63"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="63"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="65"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="C6" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="68"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1894,8 +2061,8 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -1906,8 +2073,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -1916,7 +2083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
@@ -1925,9 +2092,9 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -1937,7 +2104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
@@ -1949,20 +2116,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-    </row>
-    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="59"/>
+    </row>
+    <row r="17" spans="2:14" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
@@ -1975,23 +2144,29 @@
       <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="48" t="s">
+      <c r="F17" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="49" t="s">
+      <c r="H17" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
@@ -2018,11 +2193,18 @@
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K18" s="35">
+        <f>F18*J18</f>
+        <v>948.96896995071495</v>
+      </c>
+      <c r="L18" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
@@ -2048,12 +2230,19 @@
         <v>2850</v>
       </c>
       <c r="I19" s="28">
-        <f t="shared" ref="I19:I25" si="2">H19*G19</f>
+        <f>H19*G19</f>
         <v>917.7</v>
       </c>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" ref="K19:K25" si="2">F19*J19</f>
+        <v>48.962505868338646</v>
+      </c>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
@@ -2078,12 +2267,19 @@
         <v>1518</v>
       </c>
       <c r="I20" s="28">
+        <f t="shared" ref="I20:I25" si="3">H20*G20</f>
+        <v>847.0440000000001</v>
+      </c>
+      <c r="J20" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K20" s="28">
         <f t="shared" si="2"/>
-        <v>847.0440000000001</v>
-      </c>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+        <v>39.513601227080308</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
@@ -2108,12 +2304,19 @@
         <v>635</v>
       </c>
       <c r="I21" s="28">
+        <f t="shared" si="3"/>
+        <v>354.33000000000004</v>
+      </c>
+      <c r="J21" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K21" s="28">
         <f t="shared" si="2"/>
-        <v>354.33000000000004</v>
-      </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+        <v>109.09189903998259</v>
+      </c>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
@@ -2138,14 +2341,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K22" s="35">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+        <v>587.88899859279468</v>
+      </c>
+      <c r="L22" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
@@ -2170,14 +2380,21 @@
         <v>7875</v>
       </c>
       <c r="I23" s="28">
+        <f t="shared" si="3"/>
+        <v>2134.125</v>
+      </c>
+      <c r="J23" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K23" s="28">
         <f t="shared" si="2"/>
-        <v>2134.125</v>
-      </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+        <v>793.83159532206082</v>
+      </c>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="13">
         <v>0.17</v>
@@ -2200,21 +2417,28 @@
         <v>2052</v>
       </c>
       <c r="I24" s="28">
+        <f t="shared" si="3"/>
+        <v>556.09199999999998</v>
+      </c>
+      <c r="J24" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K24" s="28">
         <f t="shared" si="2"/>
-        <v>556.09199999999998</v>
-      </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+        <v>620.54949851461663</v>
+      </c>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="13">
         <f>15.39/5</f>
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="4">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2232,14 +2456,21 @@
         <v>8800</v>
       </c>
       <c r="I25" s="28">
+        <f t="shared" si="3"/>
+        <v>1980</v>
+      </c>
+      <c r="J25" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K25" s="28">
         <f t="shared" si="2"/>
-        <v>1980</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>145.1577774303197</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
         <v>22</v>
       </c>
@@ -2259,12 +2490,14 @@
         <f>$C$13-SUM(I18:I25)</f>
         <v>6612.7084000000004</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="19"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="41">
@@ -2275,21 +2508,23 @@
       <c r="F27" s="42"/>
       <c r="G27" s="43"/>
       <c r="H27" s="43">
-        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
+        <f t="shared" ref="H27:I27" si="5">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
       <c r="I27" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="44"/>
-      <c r="L27" s="1"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="44"/>
+      <c r="N27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B16:L16"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -2297,42 +2532,42 @@
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D21 D23:D25">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
       <formula>$E18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>$E22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="I26:K26">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="I27:K27">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2344,11 +2579,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07509E94-09C3-4B36-9ECC-C7D178D08A9D}">
-  <dimension ref="B2:L27"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2357,65 +2590,67 @@
     <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="21.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="61"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="64"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="63"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="63"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="65"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="C6" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="68"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2424,8 +2659,8 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -2436,8 +2671,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -2446,7 +2681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
@@ -2455,9 +2690,9 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -2467,7 +2702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
@@ -2479,20 +2714,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-    </row>
-    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="59"/>
+    </row>
+    <row r="17" spans="2:14" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
@@ -2505,23 +2742,29 @@
       <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>32</v>
+      <c r="F17" s="47" t="s">
+        <v>42</v>
       </c>
       <c r="G17" s="48" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
@@ -2548,11 +2791,18 @@
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K18" s="35">
+        <f>F18*J18</f>
+        <v>948.96896995071495</v>
+      </c>
+      <c r="L18" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
@@ -2581,9 +2831,16 @@
         <f t="shared" ref="I19:I25" si="2">H19*G19</f>
         <v>917.7</v>
       </c>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" ref="K19:K25" si="3">F19*J19</f>
+        <v>48.962505868338646</v>
+      </c>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
@@ -2611,9 +2868,16 @@
         <f t="shared" si="2"/>
         <v>847.0440000000001</v>
       </c>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J20" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" si="3"/>
+        <v>39.513601227080308</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
@@ -2641,9 +2905,16 @@
         <f t="shared" si="2"/>
         <v>354.33000000000004</v>
       </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K21" s="28">
+        <f t="shared" si="3"/>
+        <v>109.09189903998259</v>
+      </c>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
@@ -2671,11 +2942,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J22" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K22" s="35">
+        <f t="shared" si="3"/>
+        <v>587.88899859279468</v>
+      </c>
+      <c r="L22" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
@@ -2703,11 +2981,18 @@
         <f t="shared" si="2"/>
         <v>2134.125</v>
       </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J23" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K23" s="28">
+        <f t="shared" si="3"/>
+        <v>793.83159532206082</v>
+      </c>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="13">
         <v>0.17</v>
@@ -2733,18 +3018,25 @@
         <f t="shared" si="2"/>
         <v>556.09199999999998</v>
       </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J24" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K24" s="28">
+        <f t="shared" si="3"/>
+        <v>620.54949851461663</v>
+      </c>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="13">
         <f>15.39/5</f>
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="4">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2765,11 +3057,18 @@
         <f t="shared" si="2"/>
         <v>1980</v>
       </c>
-      <c r="J25" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K25" s="28">
+        <f t="shared" si="3"/>
+        <v>145.1577774303197</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
         <v>22</v>
       </c>
@@ -2789,12 +3088,14 @@
         <f>$C$13-SUM(I18:I25)</f>
         <v>6612.7084000000004</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="19"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="41">
@@ -2805,20 +3106,22 @@
       <c r="F27" s="42"/>
       <c r="G27" s="43"/>
       <c r="H27" s="43">
-        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
+        <f t="shared" ref="H27:I27" si="5">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
       <c r="I27" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="44"/>
-      <c r="L27" s="1"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="44"/>
+      <c r="N27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B16:L16"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -2827,42 +3130,52 @@
     <mergeCell ref="B8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D21 D23:D25">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="greaterThan">
       <formula>$E18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
       <formula>$E22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26:K26">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27:K27">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2874,11 +3187,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C792F2A7-A451-44D0-B4BC-456BE5420D34}">
-  <dimension ref="B2:L27"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2887,65 +3198,67 @@
     <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="71.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="21.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="61"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="64"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="63"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="63"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="65"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
+      <c r="C6" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="68"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2954,8 +3267,8 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="6">
@@ -2966,8 +3279,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="53"/>
       <c r="C11" s="6">
         <f>C10*0.09290304</f>
         <v>1659.8676480000001</v>
@@ -2976,7 +3289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
@@ -2985,9 +3298,9 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="22">
         <f>7937.1558+1673.2028+1059.217+1673.2138+1059.21</f>
@@ -2997,7 +3310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
@@ -3009,20 +3322,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-    </row>
-    <row r="17" spans="2:12" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="59"/>
+    </row>
+    <row r="17" spans="2:14" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="46" t="s">
         <v>0</v>
       </c>
@@ -3035,23 +3350,29 @@
       <c r="E17" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>32</v>
+      <c r="F17" s="47" t="s">
+        <v>42</v>
       </c>
       <c r="G17" s="48" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
@@ -3078,11 +3399,18 @@
         <f>H18*G18</f>
         <v>0</v>
       </c>
-      <c r="J18" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K18" s="35">
+        <f>F18*J18</f>
+        <v>948.96896995071495</v>
+      </c>
+      <c r="L18" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
@@ -3108,12 +3436,19 @@
         <v>2850</v>
       </c>
       <c r="I19" s="28">
-        <f t="shared" ref="I19:I25" si="2">H19*G19</f>
+        <f>H19*G19</f>
         <v>917.7</v>
       </c>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" ref="K19:K25" si="2">F19*J19</f>
+        <v>48.962505868338646</v>
+      </c>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
@@ -3138,12 +3473,19 @@
         <v>1518</v>
       </c>
       <c r="I20" s="28">
+        <f t="shared" ref="I19:I25" si="3">H20*G20</f>
+        <v>847.0440000000001</v>
+      </c>
+      <c r="J20" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K20" s="28">
         <f t="shared" si="2"/>
-        <v>847.0440000000001</v>
-      </c>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+        <v>39.513601227080308</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
@@ -3168,12 +3510,19 @@
         <v>635</v>
       </c>
       <c r="I21" s="28">
+        <f t="shared" si="3"/>
+        <v>354.33000000000004</v>
+      </c>
+      <c r="J21" s="51">
+        <v>0.85899133102348502</v>
+      </c>
+      <c r="K21" s="28">
         <f t="shared" si="2"/>
-        <v>354.33000000000004</v>
-      </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+        <v>109.09189903998259</v>
+      </c>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="31" t="s">
         <v>28</v>
       </c>
@@ -3198,14 +3547,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="52">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K22" s="35">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+        <v>587.88899859279468</v>
+      </c>
+      <c r="L22" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
@@ -3230,14 +3586,21 @@
         <v>7875</v>
       </c>
       <c r="I23" s="28">
+        <f t="shared" si="3"/>
+        <v>2134.125</v>
+      </c>
+      <c r="J23" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K23" s="28">
         <f t="shared" si="2"/>
-        <v>2134.125</v>
-      </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+        <v>793.83159532206082</v>
+      </c>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="13">
         <v>0.17</v>
@@ -3260,21 +3623,28 @@
         <v>2052</v>
       </c>
       <c r="I24" s="28">
+        <f t="shared" si="3"/>
+        <v>556.09199999999998</v>
+      </c>
+      <c r="J24" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K24" s="28">
         <f t="shared" si="2"/>
-        <v>556.09199999999998</v>
-      </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+        <v>620.54949851461663</v>
+      </c>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="13">
         <f>15.39/5</f>
         <v>3.0780000000000003</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" ref="D25" si="3">ROUND(C25*($C$10/1000),0)</f>
+        <f t="shared" ref="D25" si="4">ROUND(C25*($C$10/1000),0)</f>
         <v>55</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -3292,14 +3662,21 @@
         <v>8800</v>
       </c>
       <c r="I25" s="28">
+        <f t="shared" si="3"/>
+        <v>1980</v>
+      </c>
+      <c r="J25" s="51">
+        <v>0.90723610893949802</v>
+      </c>
+      <c r="K25" s="28">
         <f t="shared" si="2"/>
-        <v>1980</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>145.1577774303197</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
         <v>22</v>
       </c>
@@ -3319,12 +3696,14 @@
         <f>$C$13-SUM(I18:I25)</f>
         <v>6612.7084000000004</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="2:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="19"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="41">
@@ -3335,20 +3714,22 @@
       <c r="F27" s="42"/>
       <c r="G27" s="43"/>
       <c r="H27" s="43">
-        <f t="shared" ref="H27:I27" si="4">SUM(H18:H26)</f>
+        <f t="shared" ref="H27:I27" si="5">SUM(H18:H26)</f>
         <v>23730</v>
       </c>
       <c r="I27" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13401.999400000001</v>
       </c>
-      <c r="J27" s="44"/>
-      <c r="L27" s="1"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="44"/>
+      <c r="N27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B16:L16"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -3357,41 +3738,51 @@
     <mergeCell ref="B8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D21 D23:D25">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>$E18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>$E22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="G27">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="I27">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
+  <conditionalFormatting sqref="J26:K26">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
+  <conditionalFormatting sqref="J27:K27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>